<commit_message>
IYCF2 and PPCF constraint
</commit_message>
<xml_diff>
--- a/analyses/inputs/Medium 2020 base/Afghanistan_input.xlsx
+++ b/analyses/inputs/Medium 2020 base/Afghanistan_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\Nutrition\analyses\inputs\Medium 2020 base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1017E858-01FD-4DE3-935B-ADA8111A9ED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53F818DB-92C5-46B5-822A-F90C3685970F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17196" yWindow="-13068" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="15" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -6678,8 +6678,8 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6744,9 +6744,7 @@
       <c r="B6" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="87" t="s">
-        <v>58</v>
-      </c>
+      <c r="C6" s="87"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
@@ -12900,12 +12898,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12915,6 +12907,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -18790,7 +18788,7 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="B10:F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>